<commit_message>
benchmarked with 10k nodes
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="63">
   <si>
     <t>Prim's algorithm results</t>
   </si>
@@ -38,118 +38,169 @@
     <t>Binary Heap</t>
   </si>
   <si>
-    <t>11.11</t>
+    <t>11.52</t>
   </si>
   <si>
     <t>Strict Fibonacci Heap</t>
   </si>
   <si>
-    <t>33.86</t>
+    <t>34.22</t>
   </si>
   <si>
     <t>0.5</t>
   </si>
   <si>
-    <t>56.93</t>
-  </si>
-  <si>
-    <t>20.12</t>
+    <t>47.27</t>
+  </si>
+  <si>
+    <t>21.75</t>
   </si>
   <si>
     <t>0.9</t>
   </si>
   <si>
-    <t>28.53</t>
-  </si>
-  <si>
-    <t>33.51</t>
+    <t>29.91</t>
+  </si>
+  <si>
+    <t>31.67</t>
   </si>
   <si>
     <t>1.0</t>
   </si>
   <si>
-    <t>31.30</t>
-  </si>
-  <si>
-    <t>34.17</t>
+    <t>31.98</t>
+  </si>
+  <si>
+    <t>34.75</t>
   </si>
   <si>
     <t>5000</t>
   </si>
   <si>
-    <t>144.01</t>
-  </si>
-  <si>
-    <t>155.74</t>
-  </si>
-  <si>
-    <t>317.46</t>
-  </si>
-  <si>
-    <t>332.72</t>
-  </si>
-  <si>
-    <t>511.18</t>
-  </si>
-  <si>
-    <t>521.50</t>
-  </si>
-  <si>
-    <t>628.45</t>
-  </si>
-  <si>
-    <t>629.63</t>
+    <t>161.23</t>
+  </si>
+  <si>
+    <t>151.01</t>
+  </si>
+  <si>
+    <t>340.53</t>
+  </si>
+  <si>
+    <t>352.41</t>
+  </si>
+  <si>
+    <t>566.32</t>
+  </si>
+  <si>
+    <t>568.64</t>
+  </si>
+  <si>
+    <t>673.28</t>
+  </si>
+  <si>
+    <t>672.59</t>
+  </si>
+  <si>
+    <t>10000</t>
+  </si>
+  <si>
+    <t>652.50</t>
+  </si>
+  <si>
+    <t>668.32</t>
+  </si>
+  <si>
+    <t>1472.65</t>
+  </si>
+  <si>
+    <t>1476.25</t>
+  </si>
+  <si>
+    <t>2843.10</t>
+  </si>
+  <si>
+    <t>2836.90</t>
+  </si>
+  <si>
+    <t>3119.65</t>
+  </si>
+  <si>
+    <t>3083.64</t>
   </si>
   <si>
     <t>Dijkstra's algorithm results</t>
   </si>
   <si>
-    <t>12.56</t>
-  </si>
-  <si>
-    <t>17.85</t>
-  </si>
-  <si>
-    <t>11.93</t>
-  </si>
-  <si>
-    <t>22.39</t>
-  </si>
-  <si>
-    <t>25.98</t>
-  </si>
-  <si>
-    <t>31.14</t>
-  </si>
-  <si>
-    <t>27.39</t>
-  </si>
-  <si>
-    <t>30.85</t>
-  </si>
-  <si>
-    <t>134.77</t>
-  </si>
-  <si>
-    <t>161.21</t>
-  </si>
-  <si>
-    <t>298.24</t>
-  </si>
-  <si>
-    <t>327.49</t>
-  </si>
-  <si>
-    <t>449.70</t>
-  </si>
-  <si>
-    <t>479.84</t>
-  </si>
-  <si>
-    <t>580.70</t>
-  </si>
-  <si>
-    <t>614.16</t>
+    <t>14.10</t>
+  </si>
+  <si>
+    <t>18.61</t>
+  </si>
+  <si>
+    <t>11.20</t>
+  </si>
+  <si>
+    <t>19.58</t>
+  </si>
+  <si>
+    <t>27.14</t>
+  </si>
+  <si>
+    <t>31.36</t>
+  </si>
+  <si>
+    <t>30.04</t>
+  </si>
+  <si>
+    <t>32.54</t>
+  </si>
+  <si>
+    <t>145.62</t>
+  </si>
+  <si>
+    <t>171.01</t>
+  </si>
+  <si>
+    <t>334.95</t>
+  </si>
+  <si>
+    <t>363.91</t>
+  </si>
+  <si>
+    <t>513.14</t>
+  </si>
+  <si>
+    <t>557.15</t>
+  </si>
+  <si>
+    <t>525.38</t>
+  </si>
+  <si>
+    <t>558.53</t>
+  </si>
+  <si>
+    <t>718.70</t>
+  </si>
+  <si>
+    <t>777.00</t>
+  </si>
+  <si>
+    <t>1448.34</t>
+  </si>
+  <si>
+    <t>1572.81</t>
+  </si>
+  <si>
+    <t>2549.24</t>
+  </si>
+  <si>
+    <t>2685.74</t>
+  </si>
+  <si>
+    <t>2918.11</t>
+  </si>
+  <si>
+    <t>3055.02</t>
   </si>
 </sst>
 </file>
@@ -194,14 +245,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="22.96484375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="4.9140625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="5.9140625" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="3.3828125" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="18.078125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="7.5" customWidth="true" bestFit="true"/>
@@ -450,140 +501,140 @@
         <v>28</v>
       </c>
     </row>
+    <row r="19">
+      <c r="B19" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="C19" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D19" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="E19" t="s" s="0">
+        <v>30</v>
+      </c>
+    </row>
     <row r="20">
-      <c r="A20" t="s" s="0">
-        <v>29</v>
+      <c r="B20" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="C20" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D20" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E20" t="s" s="0">
+        <v>31</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" t="s" s="0">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C21" t="s" s="0">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D21" t="s" s="0">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E21" t="s" s="0">
-        <v>4</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" t="s" s="0">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="C22" t="s" s="0">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D22" t="s" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E22" t="s" s="0">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" t="s" s="0">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="C23" t="s" s="0">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D23" t="s" s="0">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E23" t="s" s="0">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" t="s" s="0">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="C24" t="s" s="0">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D24" t="s" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E24" t="s" s="0">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25">
       <c r="B25" t="s" s="0">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="C25" t="s" s="0">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D25" t="s" s="0">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E25" t="s" s="0">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" t="s" s="0">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="C26" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D26" t="s" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E26" t="s" s="0">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="B27" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="C27" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="D27" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="E27" t="s" s="0">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28">
-      <c r="B28" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="C28" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="D28" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="E28" t="s" s="0">
-        <v>36</v>
+      <c r="A28" t="s" s="0">
+        <v>38</v>
       </c>
     </row>
     <row r="29">
       <c r="B29" t="s" s="0">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C29" t="s" s="0">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D29" t="s" s="0">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E29" t="s" s="0">
-        <v>37</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" t="s" s="0">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C30" t="s" s="0">
         <v>6</v>
@@ -592,12 +643,12 @@
         <v>7</v>
       </c>
       <c r="E30" t="s" s="0">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31">
       <c r="B31" t="s" s="0">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C31" t="s" s="0">
         <v>6</v>
@@ -606,12 +657,12 @@
         <v>9</v>
       </c>
       <c r="E31" t="s" s="0">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32">
       <c r="B32" t="s" s="0">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C32" t="s" s="0">
         <v>11</v>
@@ -620,12 +671,12 @@
         <v>7</v>
       </c>
       <c r="E32" t="s" s="0">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33">
       <c r="B33" t="s" s="0">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C33" t="s" s="0">
         <v>11</v>
@@ -634,12 +685,12 @@
         <v>9</v>
       </c>
       <c r="E33" t="s" s="0">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34">
       <c r="B34" t="s" s="0">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C34" t="s" s="0">
         <v>14</v>
@@ -648,12 +699,12 @@
         <v>7</v>
       </c>
       <c r="E34" t="s" s="0">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="35">
       <c r="B35" t="s" s="0">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C35" t="s" s="0">
         <v>14</v>
@@ -662,12 +713,12 @@
         <v>9</v>
       </c>
       <c r="E35" t="s" s="0">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="36">
       <c r="B36" t="s" s="0">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C36" t="s" s="0">
         <v>17</v>
@@ -676,12 +727,12 @@
         <v>7</v>
       </c>
       <c r="E36" t="s" s="0">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37">
       <c r="B37" t="s" s="0">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C37" t="s" s="0">
         <v>17</v>
@@ -690,7 +741,231 @@
         <v>9</v>
       </c>
       <c r="E37" t="s" s="0">
-        <v>45</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="B38" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C38" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D38" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="E38" t="s" s="0">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="B39" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C39" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D39" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E39" t="s" s="0">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="B40" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C40" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="D40" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="E40" t="s" s="0">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="B41" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C41" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="D41" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E41" t="s" s="0">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="B42" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C42" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="D42" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="E42" t="s" s="0">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="B43" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C43" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="D43" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E43" t="s" s="0">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="B44" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C44" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="D44" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="E44" t="s" s="0">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="B45" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C45" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="D45" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E45" t="s" s="0">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="B46" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="C46" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D46" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="E46" t="s" s="0">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="B47" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="C47" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D47" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E47" t="s" s="0">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="B48" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="C48" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="D48" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="E48" t="s" s="0">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="B49" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="C49" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="D49" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E49" t="s" s="0">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="B50" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="C50" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="D50" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="E50" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="B51" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="C51" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="D51" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E51" t="s" s="0">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="B52" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="C52" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="D52" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="E52" t="s" s="0">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="B53" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="C53" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="D53" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E53" t="s" s="0">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>